<commit_message>
first ticketing system script
</commit_message>
<xml_diff>
--- a/Tenant Master.xlsx
+++ b/Tenant Master.xlsx
@@ -212,7 +212,7 @@
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.21"/>
   </cols>
@@ -282,7 +282,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -322,7 +322,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -383,10 +383,10 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>